<commit_message>
added search-search form and media rules
</commit_message>
<xml_diff>
--- a/24-10-2018.xlsx
+++ b/24-10-2018.xlsx
@@ -8,13 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="3" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Лист2!$A$1:$M$48</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
   <si>
     <t>main-content</t>
   </si>
@@ -279,19 +283,38 @@
   </si>
   <si>
     <t>message-form__button</t>
+  </si>
+  <si>
+    <t>forum-search</t>
+  </si>
+  <si>
+    <t>forum-search__icon</t>
+  </si>
+  <si>
+    <t>search-icon</t>
+  </si>
+  <si>
+    <t>message-form__container</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -345,33 +368,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -384,6 +410,994 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7772400" cy="8247141"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7772400" cy="8247141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Прямоугольник 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276850" y="2162175"/>
+          <a:ext cx="1739900" cy="1949450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Прямоугольник 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4972050" y="1530350"/>
+          <a:ext cx="1762125" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Прямоугольник 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="7562850"/>
+          <a:ext cx="7658100" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Прямоугольник 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="2190750"/>
+          <a:ext cx="4495800" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Прямоугольник 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="111125" y="63500"/>
+          <a:ext cx="7556500" cy="222250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Прямоугольник 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="727075" y="3432174"/>
+          <a:ext cx="3956050" cy="1165225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Прямоугольник 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495299" y="3549650"/>
+          <a:ext cx="4473575" cy="3124200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Соединительная линия уступом 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5362575" y="4362450"/>
+          <a:ext cx="1752600" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Соединительная линия уступом 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4638675" y="5153025"/>
+          <a:ext cx="2486025" cy="2400300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155573</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292103</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>63503</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Соединительная линия уступом 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4033837" y="1455737"/>
+          <a:ext cx="4622805" cy="2371727"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 36607"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1284582" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="5219700"/>
+          <a:ext cx="1284582" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>переиспользовать</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47629</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Соединительная линия уступом 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1809750" y="1038228"/>
+          <a:ext cx="1571626" cy="1181101"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="578813" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="885825"/>
+          <a:ext cx="578813" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>готово</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Соединительная линия уступом 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5016500" y="6543675"/>
+          <a:ext cx="406400" cy="107950"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Соединительная линия уступом 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6038850" y="1657350"/>
+          <a:ext cx="695325" cy="4597400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -83105"/>
+            <a:gd name="adj2" fmla="val 60704"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Соединительная линия уступом 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3789363" y="4735512"/>
+          <a:ext cx="1647824" cy="1511300"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="961289" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6638925" y="6505575"/>
+          <a:ext cx="961289" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>новые блоки</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K87"/>
+  <dimension ref="A2:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,7 +2741,7 @@
         <v>83</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f t="shared" ref="G85:G87" si="5">A85&amp;B85&amp;C85&amp;D85&amp;E85</f>
+        <f t="shared" ref="G85:G97" si="5">A85&amp;B85&amp;C85&amp;D85&amp;E85</f>
         <v>message-form</v>
       </c>
       <c r="I85" s="1" t="s">
@@ -1742,14 +2756,14 @@
         <v>24</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>message-form__input</v>
+        <f t="shared" ref="G86" si="6">A86&amp;B86&amp;C86&amp;D86&amp;E86</f>
+        <v>message-form__container</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,19 +2773,144 @@
       <c r="B87" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>85</v>
+      <c r="C87" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="G87" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>message-form__input</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G88" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>message-form__button</v>
       </c>
-      <c r="I87" s="1" t="s">
+      <c r="I88" s="1" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G89" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G90" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>forum-search</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G91" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>forum-search__input</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G92" s="1" t="str">
+        <f t="shared" ref="G92" si="7">A92&amp;B92&amp;C92&amp;D92&amp;E92</f>
+        <v>forum-search__icon</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="G93" s="1" t="str">
+        <f>A93&amp;B93&amp;C93&amp;D93&amp;E93</f>
+        <v>search-icon</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G94" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G95" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G96" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>